<commit_message>
Cập nhật các tính năng cho main, splitData, .xlsx
</commit_message>
<xml_diff>
--- a/Neural Network/dataModelRegression.xlsx
+++ b/Neural Network/dataModelRegression.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SimPhaHoai\Desktop\congViec_06_05_23\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SimPhaHoai\Desktop\source\congViec_06_05_23\_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -21,6 +21,26 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+  <si>
+    <t>X1</t>
+  </si>
+  <si>
+    <t>X2</t>
+  </si>
+  <si>
+    <t>X3</t>
+  </si>
+  <si>
+    <t>X4</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -342,10 +362,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E63"/>
+  <dimension ref="A1:E64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -354,20 +374,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="1">
-        <v>15</v>
-      </c>
-      <c r="B1" s="1">
-        <v>0.2</v>
-      </c>
-      <c r="C1" s="1">
-        <v>0.1</v>
-      </c>
-      <c r="D1" s="1">
-        <v>200</v>
-      </c>
-      <c r="E1" s="2">
-        <v>1.536</v>
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -378,13 +398,13 @@
         <v>0.2</v>
       </c>
       <c r="C2" s="1">
-        <v>0.3</v>
+        <v>0.1</v>
       </c>
       <c r="D2" s="1">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="E2" s="2">
-        <v>1.258</v>
+        <v>1.536</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -398,10 +418,10 @@
         <v>0.3</v>
       </c>
       <c r="D3" s="1">
-        <v>150</v>
+        <v>100</v>
       </c>
       <c r="E3" s="2">
-        <v>1.764</v>
+        <v>1.258</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -415,10 +435,10 @@
         <v>0.3</v>
       </c>
       <c r="D4" s="1">
-        <v>200</v>
+        <v>150</v>
       </c>
       <c r="E4" s="2">
-        <v>1.8540000000000001</v>
+        <v>1.764</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -429,13 +449,13 @@
         <v>0.2</v>
       </c>
       <c r="C5" s="1">
-        <v>0.5</v>
+        <v>0.3</v>
       </c>
       <c r="D5" s="1">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="E5" s="2">
-        <v>1.875</v>
+        <v>1.8540000000000001</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -449,10 +469,10 @@
         <v>0.5</v>
       </c>
       <c r="D6" s="1">
-        <v>150</v>
+        <v>100</v>
       </c>
       <c r="E6" s="2">
-        <v>2.0070000000000001</v>
+        <v>1.875</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -466,10 +486,10 @@
         <v>0.5</v>
       </c>
       <c r="D7" s="1">
-        <v>200</v>
+        <v>150</v>
       </c>
       <c r="E7" s="2">
-        <v>2.2040000000000002</v>
+        <v>2.0070000000000001</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -477,16 +497,16 @@
         <v>15</v>
       </c>
       <c r="B8" s="1">
-        <v>0.4</v>
+        <v>0.2</v>
       </c>
       <c r="C8" s="1">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="D8" s="1">
-        <v>150</v>
+        <v>200</v>
       </c>
       <c r="E8" s="2">
-        <v>1.593</v>
+        <v>2.2040000000000002</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -500,10 +520,10 @@
         <v>0.1</v>
       </c>
       <c r="D9" s="1">
-        <v>200</v>
+        <v>150</v>
       </c>
       <c r="E9" s="2">
-        <v>1.6439999999999999</v>
+        <v>1.593</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -514,13 +534,13 @@
         <v>0.4</v>
       </c>
       <c r="C10" s="1">
-        <v>0.3</v>
+        <v>0.1</v>
       </c>
       <c r="D10" s="1">
         <v>200</v>
       </c>
       <c r="E10" s="2">
-        <v>1.8680000000000001</v>
+        <v>1.6439999999999999</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -531,13 +551,13 @@
         <v>0.4</v>
       </c>
       <c r="C11" s="1">
-        <v>0.5</v>
+        <v>0.3</v>
       </c>
       <c r="D11" s="1">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="E11" s="2">
-        <v>2.1070000000000002</v>
+        <v>1.8680000000000001</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -551,10 +571,10 @@
         <v>0.5</v>
       </c>
       <c r="D12" s="1">
-        <v>150</v>
+        <v>100</v>
       </c>
       <c r="E12" s="2">
-        <v>2.29</v>
+        <v>2.1070000000000002</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -568,10 +588,10 @@
         <v>0.5</v>
       </c>
       <c r="D13" s="1">
-        <v>200</v>
+        <v>150</v>
       </c>
       <c r="E13" s="2">
-        <v>2.1320000000000001</v>
+        <v>2.29</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -579,16 +599,16 @@
         <v>15</v>
       </c>
       <c r="B14" s="1">
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
       <c r="C14" s="1">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="D14" s="1">
-        <v>150</v>
+        <v>200</v>
       </c>
       <c r="E14" s="2">
-        <v>1.6890000000000001</v>
+        <v>2.1320000000000001</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -602,10 +622,10 @@
         <v>0.1</v>
       </c>
       <c r="D15" s="1">
-        <v>200</v>
+        <v>150</v>
       </c>
       <c r="E15" s="2">
-        <v>1.839</v>
+        <v>1.6890000000000001</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -616,13 +636,13 @@
         <v>0.6</v>
       </c>
       <c r="C16" s="1">
-        <v>0.3</v>
+        <v>0.1</v>
       </c>
       <c r="D16" s="1">
-        <v>150</v>
+        <v>200</v>
       </c>
       <c r="E16" s="2">
-        <v>1.7969999999999999</v>
+        <v>1.839</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -636,10 +656,10 @@
         <v>0.3</v>
       </c>
       <c r="D17" s="1">
-        <v>200</v>
+        <v>150</v>
       </c>
       <c r="E17" s="2">
-        <v>1.7949999999999999</v>
+        <v>1.7969999999999999</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -650,30 +670,30 @@
         <v>0.6</v>
       </c>
       <c r="C18" s="1">
-        <v>0.5</v>
+        <v>0.3</v>
       </c>
       <c r="D18" s="1">
-        <v>150</v>
+        <v>200</v>
       </c>
       <c r="E18" s="2">
-        <v>2.5070000000000001</v>
+        <v>1.7949999999999999</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="B19" s="1">
-        <v>0.2</v>
+        <v>0.6</v>
       </c>
       <c r="C19" s="1">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="D19" s="1">
-        <v>100</v>
+        <v>150</v>
       </c>
       <c r="E19" s="2">
-        <v>2.403</v>
+        <v>2.5070000000000001</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -684,13 +704,13 @@
         <v>0.2</v>
       </c>
       <c r="C20" s="1">
-        <v>0.3</v>
+        <v>0.1</v>
       </c>
       <c r="D20" s="1">
         <v>100</v>
       </c>
       <c r="E20" s="2">
-        <v>2.3719999999999999</v>
+        <v>2.403</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -704,10 +724,10 @@
         <v>0.3</v>
       </c>
       <c r="D21" s="1">
-        <v>150</v>
+        <v>100</v>
       </c>
       <c r="E21" s="2">
-        <v>2.1669999999999998</v>
+        <v>2.3719999999999999</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -718,13 +738,13 @@
         <v>0.2</v>
       </c>
       <c r="C22" s="1">
-        <v>0.5</v>
+        <v>0.3</v>
       </c>
       <c r="D22" s="1">
-        <v>100</v>
+        <v>150</v>
       </c>
       <c r="E22" s="2">
-        <v>2.0390000000000001</v>
+        <v>2.1669999999999998</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -732,16 +752,16 @@
         <v>25</v>
       </c>
       <c r="B23" s="1">
-        <v>0.4</v>
+        <v>0.2</v>
       </c>
       <c r="C23" s="1">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="D23" s="1">
         <v>100</v>
       </c>
       <c r="E23" s="2">
-        <v>2.218</v>
+        <v>2.0390000000000001</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -755,10 +775,10 @@
         <v>0.1</v>
       </c>
       <c r="D24" s="1">
-        <v>150</v>
+        <v>100</v>
       </c>
       <c r="E24" s="2">
-        <v>2.3490000000000002</v>
+        <v>2.218</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -772,10 +792,10 @@
         <v>0.1</v>
       </c>
       <c r="D25" s="1">
-        <v>200</v>
+        <v>150</v>
       </c>
       <c r="E25" s="2">
-        <v>2.4140000000000001</v>
+        <v>2.3490000000000002</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -786,13 +806,13 @@
         <v>0.4</v>
       </c>
       <c r="C26" s="1">
-        <v>0.3</v>
+        <v>0.1</v>
       </c>
       <c r="D26" s="1">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="E26" s="2">
-        <v>2.0249999999999999</v>
+        <v>2.4140000000000001</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
@@ -806,10 +826,10 @@
         <v>0.3</v>
       </c>
       <c r="D27" s="1">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="E27" s="2">
-        <v>1.964</v>
+        <v>2.0249999999999999</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
@@ -820,13 +840,13 @@
         <v>0.4</v>
       </c>
       <c r="C28" s="1">
-        <v>0.5</v>
+        <v>0.3</v>
       </c>
       <c r="D28" s="1">
-        <v>150</v>
+        <v>200</v>
       </c>
       <c r="E28" s="2">
-        <v>2.2999999999999998</v>
+        <v>1.964</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -840,10 +860,10 @@
         <v>0.5</v>
       </c>
       <c r="D29" s="1">
-        <v>200</v>
+        <v>150</v>
       </c>
       <c r="E29" s="2">
-        <v>2.1459999999999999</v>
+        <v>2.2999999999999998</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
@@ -851,16 +871,16 @@
         <v>25</v>
       </c>
       <c r="B30" s="1">
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
       <c r="C30" s="1">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="D30" s="1">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="E30" s="2">
-        <v>2.214</v>
+        <v>2.1459999999999999</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
@@ -874,10 +894,10 @@
         <v>0.1</v>
       </c>
       <c r="D31" s="1">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="E31" s="2">
-        <v>2.036</v>
+        <v>2.214</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
@@ -888,13 +908,13 @@
         <v>0.6</v>
       </c>
       <c r="C32" s="1">
-        <v>0.3</v>
+        <v>0.1</v>
       </c>
       <c r="D32" s="1">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="E32" s="2">
-        <v>2.1549999999999998</v>
+        <v>2.036</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
@@ -908,10 +928,10 @@
         <v>0.3</v>
       </c>
       <c r="D33" s="1">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="E33" s="2">
-        <v>2.0070000000000001</v>
+        <v>2.1549999999999998</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
@@ -922,13 +942,13 @@
         <v>0.6</v>
       </c>
       <c r="C34" s="1">
-        <v>0.5</v>
+        <v>0.3</v>
       </c>
       <c r="D34" s="1">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="E34" s="2">
-        <v>2.464</v>
+        <v>2.0070000000000001</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
@@ -942,10 +962,10 @@
         <v>0.5</v>
       </c>
       <c r="D35" s="1">
-        <v>150</v>
+        <v>100</v>
       </c>
       <c r="E35" s="2">
-        <v>2.036</v>
+        <v>2.464</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
@@ -959,27 +979,27 @@
         <v>0.5</v>
       </c>
       <c r="D36" s="1">
-        <v>200</v>
+        <v>150</v>
       </c>
       <c r="E36" s="2">
-        <v>2.2400000000000002</v>
+        <v>2.036</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="B37" s="1">
-        <v>0.2</v>
+        <v>0.6</v>
       </c>
       <c r="C37" s="1">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="D37" s="1">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="E37" s="2">
-        <v>1.897</v>
+        <v>2.2400000000000002</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
@@ -993,10 +1013,10 @@
         <v>0.1</v>
       </c>
       <c r="D38" s="1">
-        <v>150</v>
+        <v>100</v>
       </c>
       <c r="E38" s="2">
-        <v>2.222</v>
+        <v>1.897</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
@@ -1010,10 +1030,10 @@
         <v>0.1</v>
       </c>
       <c r="D39" s="1">
-        <v>200</v>
+        <v>150</v>
       </c>
       <c r="E39" s="2">
-        <v>2.4</v>
+        <v>2.222</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
@@ -1024,13 +1044,13 @@
         <v>0.2</v>
       </c>
       <c r="C40" s="1">
-        <v>0.3</v>
+        <v>0.1</v>
       </c>
       <c r="D40" s="1">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="E40" s="2">
-        <v>1.5109999999999999</v>
+        <v>2.4</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
@@ -1041,13 +1061,13 @@
         <v>0.2</v>
       </c>
       <c r="C41" s="1">
-        <v>0.5</v>
+        <v>0.3</v>
       </c>
       <c r="D41" s="1">
         <v>100</v>
       </c>
       <c r="E41" s="2">
-        <v>2.032</v>
+        <v>1.5109999999999999</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
@@ -1061,10 +1081,10 @@
         <v>0.5</v>
       </c>
       <c r="D42" s="1">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="E42" s="2">
-        <v>2.2629999999999999</v>
+        <v>2.032</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
@@ -1072,16 +1092,16 @@
         <v>35</v>
       </c>
       <c r="B43" s="1">
-        <v>0.4</v>
+        <v>0.2</v>
       </c>
       <c r="C43" s="1">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="D43" s="1">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="E43" s="2">
-        <v>1.6859999999999999</v>
+        <v>2.2629999999999999</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
@@ -1095,10 +1115,10 @@
         <v>0.1</v>
       </c>
       <c r="D44" s="1">
-        <v>150</v>
+        <v>100</v>
       </c>
       <c r="E44" s="2">
-        <v>2.25</v>
+        <v>1.6859999999999999</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
@@ -1109,13 +1129,13 @@
         <v>0.4</v>
       </c>
       <c r="C45" s="1">
-        <v>0.3</v>
+        <v>0.1</v>
       </c>
       <c r="D45" s="1">
-        <v>100</v>
+        <v>150</v>
       </c>
       <c r="E45" s="2">
-        <v>2.1139999999999999</v>
+        <v>2.25</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
@@ -1129,10 +1149,10 @@
         <v>0.3</v>
       </c>
       <c r="D46" s="1">
-        <v>150</v>
+        <v>100</v>
       </c>
       <c r="E46" s="2">
-        <v>1.875</v>
+        <v>2.1139999999999999</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
@@ -1143,13 +1163,13 @@
         <v>0.4</v>
       </c>
       <c r="C47" s="1">
-        <v>0.5</v>
+        <v>0.3</v>
       </c>
       <c r="D47" s="1">
         <v>150</v>
       </c>
       <c r="E47" s="2">
-        <v>2.1429999999999998</v>
+        <v>1.875</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
@@ -1163,10 +1183,10 @@
         <v>0.5</v>
       </c>
       <c r="D48" s="1">
-        <v>200</v>
+        <v>150</v>
       </c>
       <c r="E48" s="2">
-        <v>2.1970000000000001</v>
+        <v>2.1429999999999998</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
@@ -1174,16 +1194,16 @@
         <v>35</v>
       </c>
       <c r="B49" s="1">
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
       <c r="C49" s="1">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="D49" s="1">
-        <v>150</v>
+        <v>200</v>
       </c>
       <c r="E49" s="2">
-        <v>2.1819999999999999</v>
+        <v>2.1970000000000001</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
@@ -1197,10 +1217,10 @@
         <v>0.1</v>
       </c>
       <c r="D50" s="1">
-        <v>200</v>
+        <v>150</v>
       </c>
       <c r="E50" s="2">
-        <v>1.9470000000000001</v>
+        <v>2.1819999999999999</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
@@ -1211,13 +1231,13 @@
         <v>0.6</v>
       </c>
       <c r="C51" s="1">
-        <v>0.3</v>
+        <v>0.1</v>
       </c>
       <c r="D51" s="1">
-        <v>150</v>
+        <v>200</v>
       </c>
       <c r="E51" s="2">
-        <v>1.736</v>
+        <v>1.9470000000000001</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
@@ -1231,10 +1251,10 @@
         <v>0.3</v>
       </c>
       <c r="D52" s="1">
-        <v>200</v>
+        <v>150</v>
       </c>
       <c r="E52" s="2">
-        <v>1.8859999999999999</v>
+        <v>1.736</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
@@ -1245,13 +1265,13 @@
         <v>0.6</v>
       </c>
       <c r="C53" s="1">
-        <v>0.5</v>
+        <v>0.3</v>
       </c>
       <c r="D53" s="1">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="E53" s="2">
-        <v>2.1789999999999998</v>
+        <v>1.8859999999999999</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
@@ -1265,27 +1285,27 @@
         <v>0.5</v>
       </c>
       <c r="D54" s="1">
-        <v>150</v>
+        <v>100</v>
       </c>
       <c r="E54" s="2">
-        <v>2.1139999999999999</v>
+        <v>2.1789999999999998</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
-        <v>15</v>
+        <v>35</v>
       </c>
       <c r="B55" s="1">
-        <v>0.2</v>
+        <v>0.6</v>
       </c>
       <c r="C55" s="1">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="D55" s="1">
-        <v>100</v>
+        <v>150</v>
       </c>
       <c r="E55" s="2">
-        <v>1.754</v>
+        <v>2.1139999999999999</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
@@ -1293,16 +1313,16 @@
         <v>15</v>
       </c>
       <c r="B56" s="1">
-        <v>0.4</v>
+        <v>0.2</v>
       </c>
       <c r="C56" s="1">
-        <v>0.3</v>
+        <v>0.1</v>
       </c>
       <c r="D56" s="1">
-        <v>150</v>
+        <v>100</v>
       </c>
       <c r="E56" s="2">
-        <v>1.5109999999999999</v>
+        <v>1.754</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
@@ -1310,33 +1330,33 @@
         <v>15</v>
       </c>
       <c r="B57" s="1">
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
       <c r="C57" s="1">
-        <v>0.5</v>
+        <v>0.3</v>
       </c>
       <c r="D57" s="1">
-        <v>200</v>
+        <v>150</v>
       </c>
       <c r="E57" s="2">
-        <v>2.3149999999999999</v>
+        <v>1.5109999999999999</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="B58" s="1">
-        <v>0.2</v>
+        <v>0.6</v>
       </c>
       <c r="C58" s="1">
-        <v>0.3</v>
+        <v>0.5</v>
       </c>
       <c r="D58" s="1">
         <v>200</v>
       </c>
       <c r="E58" s="2">
-        <v>2.1680000000000001</v>
+        <v>2.3149999999999999</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
@@ -1344,16 +1364,16 @@
         <v>25</v>
       </c>
       <c r="B59" s="1">
-        <v>0.4</v>
+        <v>0.2</v>
       </c>
       <c r="C59" s="1">
-        <v>0.5</v>
+        <v>0.3</v>
       </c>
       <c r="D59" s="1">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="E59" s="2">
-        <v>2.0539999999999998</v>
+        <v>2.1680000000000001</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
@@ -1361,33 +1381,33 @@
         <v>25</v>
       </c>
       <c r="B60" s="1">
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
       <c r="C60" s="1">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="D60" s="1">
-        <v>150</v>
+        <v>100</v>
       </c>
       <c r="E60" s="2">
-        <v>2.0680000000000001</v>
+        <v>2.0539999999999998</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="B61" s="1">
-        <v>0.2</v>
+        <v>0.6</v>
       </c>
       <c r="C61" s="1">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="D61" s="1">
         <v>150</v>
       </c>
       <c r="E61" s="2">
-        <v>2.2069999999999999</v>
+        <v>2.0680000000000001</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
@@ -1395,16 +1415,16 @@
         <v>35</v>
       </c>
       <c r="B62" s="1">
-        <v>0.4</v>
+        <v>0.2</v>
       </c>
       <c r="C62" s="1">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="D62" s="1">
-        <v>200</v>
+        <v>150</v>
       </c>
       <c r="E62" s="2">
-        <v>2.5459999999999998</v>
+        <v>2.2069999999999999</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
@@ -1412,15 +1432,32 @@
         <v>35</v>
       </c>
       <c r="B63" s="1">
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
       <c r="C63" s="1">
-        <v>0.3</v>
+        <v>0.1</v>
       </c>
       <c r="D63" s="1">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="E63" s="2">
+        <v>2.5459999999999998</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A64" s="1">
+        <v>35</v>
+      </c>
+      <c r="B64" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="C64" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="D64" s="1">
+        <v>100</v>
+      </c>
+      <c r="E64" s="2">
         <v>2.1800000000000002</v>
       </c>
     </row>

</xml_diff>